<commit_message>
Primeiro commit - 04/12/2020
</commit_message>
<xml_diff>
--- a/planejamento/modelos_excel/planilha_horas_geral.xlsx
+++ b/planejamento/modelos_excel/planilha_horas_geral.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\dvmsys\planejamento\modelos_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Developer\XAMPP\htdocs\erp_sistema\planejamento\modelos_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="3975" windowWidth="20280" windowHeight="4035"/>
+    <workbookView xWindow="-15" yWindow="3975" windowWidth="20280" windowHeight="4035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="1" r:id="rId1"/>
@@ -172,8 +172,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="000000"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="000000"/>
   </numFmts>
   <fonts count="23" x14ac:knownFonts="1">
     <font>
@@ -878,7 +878,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="44" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -890,7 +890,7 @@
     <xf numFmtId="4" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="32"/>
@@ -902,6 +902,39 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="21" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="21" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -945,75 +978,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="21" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Ênfase1" xfId="9" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase2" xfId="13" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase3" xfId="17" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase4" xfId="21" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase5" xfId="25" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Ênfase6" xfId="29" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase1" xfId="10" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase2" xfId="14" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase3" xfId="18" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase4" xfId="22" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase5" xfId="26" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Ênfase6" xfId="30" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase1" xfId="11" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase2" xfId="15" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase3" xfId="19" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase4" xfId="23" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase5" xfId="27" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Ênfase6" xfId="31" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bom" xfId="1" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Cor1" xfId="9" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Cor2" xfId="13" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Cor3" xfId="17" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Cor4" xfId="21" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Cor5" xfId="25" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Cor6" xfId="29" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Cor1" xfId="10" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Cor2" xfId="14" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Cor3" xfId="18" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Cor4" xfId="22" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Cor5" xfId="26" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Cor6" xfId="30" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Cor1" xfId="11" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Cor2" xfId="15" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Cor3" xfId="19" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Cor4" xfId="23" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Cor5" xfId="27" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Cor6" xfId="31" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="6" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Célula de Verificação" xfId="7" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Célula Vinculada 2" xfId="38"/>
-    <cellStyle name="Ênfase1" xfId="8" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Ênfase2" xfId="12" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Ênfase3" xfId="16" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Ênfase4" xfId="20" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Ênfase5" xfId="24" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Ênfase6" xfId="28" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Cor1" xfId="8" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Cor2" xfId="12" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Cor3" xfId="16" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Cor4" xfId="20" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Cor5" xfId="24" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Cor6" xfId="28" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Correto" xfId="1" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Entrada" xfId="4" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutra" xfId="3" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="3" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="32"/>
     <cellStyle name="Nota 2" xfId="40"/>
@@ -1026,6 +1025,7 @@
     <cellStyle name="Título 4 2" xfId="37"/>
     <cellStyle name="Título 5" xfId="33"/>
     <cellStyle name="Total 2" xfId="42"/>
+    <cellStyle name="Verificar Célula" xfId="7" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
@@ -1099,158 +1099,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38453</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>105110</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1514475" cy="476250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 4294967295"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="0" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38453</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>105110</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1514475" cy="476250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 4294967295"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38453" y="105110"/>
-          <a:ext cx="1514475" cy="476250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38453</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>105110</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1514475" cy="476250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 4294967295"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38453" y="105110"/>
-          <a:ext cx="1514475" cy="476250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38453</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>105110</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="1514475" cy="476250"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagem 4294967295"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="38453" y="105110"/>
-          <a:ext cx="1514475" cy="476250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1542,7 +1390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
@@ -1558,124 +1406,124 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="32" t="s">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="32" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="30">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A7,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E7" s="31"/>
-      <c r="F7" s="30">
+      <c r="E7" s="17"/>
+      <c r="F7" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A7,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G7" s="31"/>
-      <c r="H7" s="30">
+      <c r="G7" s="17"/>
+      <c r="H7" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A7,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="31"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A7,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1683,26 +1531,26 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="30">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A8,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30">
+      <c r="E8" s="17"/>
+      <c r="F8" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A8,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G8" s="31"/>
-      <c r="H8" s="30">
+      <c r="G8" s="17"/>
+      <c r="H8" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A8,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I8" s="31"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A8,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1710,26 +1558,26 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="30">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A9,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="30">
+      <c r="E9" s="17"/>
+      <c r="F9" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A9,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="30">
+      <c r="G9" s="17"/>
+      <c r="H9" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A9,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="31"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A9,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1737,26 +1585,26 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="30">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A10,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E10" s="31"/>
-      <c r="F10" s="30">
+      <c r="E10" s="17"/>
+      <c r="F10" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A10,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30">
+      <c r="G10" s="17"/>
+      <c r="H10" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A10,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="31"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A10,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1764,26 +1612,26 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="30">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A11,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="31"/>
-      <c r="F11" s="30">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A11,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30">
+      <c r="G11" s="17"/>
+      <c r="H11" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A11,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="31"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A11,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1791,26 +1639,26 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="30">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A12,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E12" s="31"/>
-      <c r="F12" s="30">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A12,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30">
+      <c r="G12" s="17"/>
+      <c r="H12" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A12,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I12" s="31"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A12,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1818,26 +1666,26 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="30">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A13,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E13" s="31"/>
-      <c r="F13" s="30">
+      <c r="E13" s="17"/>
+      <c r="F13" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A13,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30">
+      <c r="G13" s="17"/>
+      <c r="H13" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A13,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I13" s="31"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A13,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1845,26 +1693,26 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="30">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A14,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="31"/>
-      <c r="F14" s="30">
+      <c r="E14" s="17"/>
+      <c r="F14" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A14,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30">
+      <c r="G14" s="17"/>
+      <c r="H14" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A14,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="31"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A14,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1872,26 +1720,26 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="30">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A15,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="31"/>
-      <c r="F15" s="30">
+      <c r="E15" s="17"/>
+      <c r="F15" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A15,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30">
+      <c r="G15" s="17"/>
+      <c r="H15" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A15,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I15" s="31"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A15,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1899,26 +1747,26 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="30">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A16,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E16" s="31"/>
-      <c r="F16" s="30">
+      <c r="E16" s="17"/>
+      <c r="F16" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A16,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G16" s="31"/>
-      <c r="H16" s="30">
+      <c r="G16" s="17"/>
+      <c r="H16" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A16,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I16" s="31"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A16,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1926,26 +1774,26 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="30">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A17,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="31"/>
-      <c r="F17" s="30">
+      <c r="E17" s="17"/>
+      <c r="F17" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A17,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30">
+      <c r="G17" s="17"/>
+      <c r="H17" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A17,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I17" s="31"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A17,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1953,26 +1801,26 @@
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="30">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A18,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E18" s="31"/>
-      <c r="F18" s="30">
+      <c r="E18" s="17"/>
+      <c r="F18" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A18,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="31"/>
-      <c r="H18" s="30">
+      <c r="G18" s="17"/>
+      <c r="H18" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A18,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="31"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A18,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -1980,26 +1828,26 @@
       <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="30">
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A19,'OS''s em execução'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E19" s="31"/>
-      <c r="F19" s="30">
+      <c r="E19" s="17"/>
+      <c r="F19" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A19,'OS''s em execução'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30">
+      <c r="G19" s="17"/>
+      <c r="H19" s="16">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A19,'OS''s em execução'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I19" s="31"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="9">
         <f ca="1">SUMIF('OS''s em execução'!$B$6:$J$10001,Resumo!A19,'OS''s em execução'!J$6:J$10001)</f>
         <v>0</v>
@@ -2007,109 +1855,109 @@
       <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" s="3" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="35"/>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="38"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="8"/>
     </row>
     <row r="21" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="30">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16">
         <f ca="1">SUM(D7:E19)</f>
         <v>0</v>
       </c>
-      <c r="E21" s="31"/>
-      <c r="F21" s="30">
+      <c r="E21" s="17"/>
+      <c r="F21" s="16">
         <f ca="1">SUM(F7:G19)</f>
         <v>0</v>
       </c>
-      <c r="G21" s="31"/>
-      <c r="H21" s="30">
+      <c r="G21" s="17"/>
+      <c r="H21" s="16">
         <f ca="1">SUM(H7:I19)</f>
         <v>0</v>
       </c>
-      <c r="I21" s="31"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="9">
         <f ca="1">SUM(J7:J19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
     </row>
     <row r="23" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="32" t="s">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="32" t="s">
+      <c r="E24" s="25"/>
+      <c r="F24" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="33"/>
-      <c r="H24" s="32" t="s">
+      <c r="G24" s="25"/>
+      <c r="H24" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I24" s="33"/>
+      <c r="I24" s="25"/>
       <c r="J24" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="30">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A25,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="30">
+      <c r="E25" s="17"/>
+      <c r="F25" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A25,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="30">
+      <c r="G25" s="17"/>
+      <c r="H25" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A25,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A25,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2117,26 +1965,26 @@
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="30">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A26,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="30">
+      <c r="E26" s="17"/>
+      <c r="F26" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A26,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30">
+      <c r="G26" s="17"/>
+      <c r="H26" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A26,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A26,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2144,26 +1992,26 @@
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="30">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A27,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="30">
+      <c r="E27" s="17"/>
+      <c r="F27" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A27,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="30">
+      <c r="G27" s="17"/>
+      <c r="H27" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A27,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I27" s="31"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A27,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2171,26 +2019,26 @@
       <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="30">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A28,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="30">
+      <c r="E28" s="17"/>
+      <c r="F28" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A28,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="30">
+      <c r="G28" s="17"/>
+      <c r="H28" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A28,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I28" s="31"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A28,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2198,26 +2046,26 @@
       <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="30">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A29,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="30">
+      <c r="E29" s="17"/>
+      <c r="F29" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A29,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G29" s="31"/>
-      <c r="H29" s="30">
+      <c r="G29" s="17"/>
+      <c r="H29" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A29,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I29" s="31"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A29,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2225,26 +2073,26 @@
       <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="30">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A30,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="30">
+      <c r="E30" s="17"/>
+      <c r="F30" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A30,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="30">
+      <c r="G30" s="17"/>
+      <c r="H30" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A30,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I30" s="31"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A30,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2252,26 +2100,26 @@
       <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="30">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A31,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="30">
+      <c r="E31" s="17"/>
+      <c r="F31" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A31,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="31"/>
-      <c r="H31" s="30">
+      <c r="G31" s="17"/>
+      <c r="H31" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A31,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I31" s="31"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A31,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2279,26 +2127,26 @@
       <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="30">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A32,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="30">
+      <c r="E32" s="17"/>
+      <c r="F32" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A32,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G32" s="31"/>
-      <c r="H32" s="30">
+      <c r="G32" s="17"/>
+      <c r="H32" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A32,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A32,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2306,26 +2154,26 @@
       <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="30">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A33,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="30">
+      <c r="E33" s="17"/>
+      <c r="F33" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A33,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="31"/>
-      <c r="H33" s="30">
+      <c r="G33" s="17"/>
+      <c r="H33" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A33,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I33" s="31"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A33,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2333,26 +2181,26 @@
       <c r="L33" s="11"/>
     </row>
     <row r="34" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="30">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A34,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="30">
+      <c r="E34" s="17"/>
+      <c r="F34" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A34,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G34" s="31"/>
-      <c r="H34" s="30">
+      <c r="G34" s="17"/>
+      <c r="H34" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A34,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I34" s="31"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A34,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2360,26 +2208,26 @@
       <c r="L34" s="11"/>
     </row>
     <row r="35" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="30">
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A35,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="30">
+      <c r="E35" s="17"/>
+      <c r="F35" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A35,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G35" s="31"/>
-      <c r="H35" s="30">
+      <c r="G35" s="17"/>
+      <c r="H35" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A35,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I35" s="31"/>
+      <c r="I35" s="17"/>
       <c r="J35" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A35,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2387,26 +2235,26 @@
       <c r="L35" s="11"/>
     </row>
     <row r="36" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="34" t="s">
+      <c r="A36" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="30">
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A36,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E36" s="31"/>
-      <c r="F36" s="30">
+      <c r="E36" s="17"/>
+      <c r="F36" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A36,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G36" s="31"/>
-      <c r="H36" s="30">
+      <c r="G36" s="17"/>
+      <c r="H36" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A36,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I36" s="31"/>
+      <c r="I36" s="17"/>
       <c r="J36" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A36,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2414,26 +2262,26 @@
       <c r="L36" s="11"/>
     </row>
     <row r="37" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="34" t="s">
+      <c r="A37" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="34"/>
-      <c r="C37" s="34"/>
-      <c r="D37" s="30">
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A37,'OS''s paralisadas'!D$6:D$10001)</f>
         <v>0</v>
       </c>
-      <c r="E37" s="31"/>
-      <c r="F37" s="30">
+      <c r="E37" s="17"/>
+      <c r="F37" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A37,'OS''s paralisadas'!F$6:F$10001)</f>
         <v>0</v>
       </c>
-      <c r="G37" s="31"/>
-      <c r="H37" s="30">
+      <c r="G37" s="17"/>
+      <c r="H37" s="16">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A37,'OS''s paralisadas'!H$6:H$10001)</f>
         <v>0</v>
       </c>
-      <c r="I37" s="31"/>
+      <c r="I37" s="17"/>
       <c r="J37" s="9">
         <f ca="1">SUMIF('OS''s paralisadas'!$B$6:$J$10001,Resumo!A37,'OS''s paralisadas'!J$6:J$10001)</f>
         <v>0</v>
@@ -2441,38 +2289,38 @@
       <c r="L37" s="11"/>
     </row>
     <row r="38" spans="1:12" s="3" customFormat="1" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35"/>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="37"/>
-      <c r="E38" s="38"/>
-      <c r="F38" s="37"/>
-      <c r="G38" s="38"/>
-      <c r="H38" s="37"/>
-      <c r="I38" s="38"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="8"/>
     </row>
     <row r="39" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="34" t="s">
+      <c r="A39" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B39" s="34"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="30">
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="16">
         <f ca="1">SUM(D25:E37)</f>
         <v>0</v>
       </c>
-      <c r="E39" s="31"/>
-      <c r="F39" s="30">
+      <c r="E39" s="17"/>
+      <c r="F39" s="16">
         <f ca="1">SUM(F25:G37)</f>
         <v>0</v>
       </c>
-      <c r="G39" s="31"/>
-      <c r="H39" s="30">
+      <c r="G39" s="17"/>
+      <c r="H39" s="16">
         <f ca="1">SUM(H25:I37)</f>
         <v>0</v>
       </c>
-      <c r="I39" s="31"/>
+      <c r="I39" s="17"/>
       <c r="J39" s="9">
         <f ca="1">SUM(J25:J37)</f>
         <v>0</v>
@@ -2488,26 +2336,26 @@
       <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:12" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="34" t="s">
+      <c r="A41" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="34"/>
-      <c r="C41" s="34"/>
-      <c r="D41" s="30">
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="16">
         <f ca="1">D39+D21</f>
         <v>0</v>
       </c>
-      <c r="E41" s="31"/>
-      <c r="F41" s="30">
+      <c r="E41" s="17"/>
+      <c r="F41" s="16">
         <f ca="1">D39+D21</f>
         <v>0</v>
       </c>
-      <c r="G41" s="31"/>
-      <c r="H41" s="30">
+      <c r="G41" s="17"/>
+      <c r="H41" s="16">
         <f ca="1">D39+D21</f>
         <v>0</v>
       </c>
-      <c r="I41" s="31"/>
+      <c r="I41" s="17"/>
       <c r="J41" s="9">
         <f ca="1">J39+J21</f>
         <v>0</v>
@@ -2515,18 +2363,111 @@
     </row>
   </sheetData>
   <mergeCells count="141">
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="D34:E34"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D37:E37"/>
     <mergeCell ref="F37:G37"/>
@@ -2551,111 +2492,18 @@
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:E19">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="equal">
@@ -2699,7 +2547,6 @@
   </conditionalFormatting>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2726,115 +2573,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="32" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="9">
         <f>F7-H7</f>
         <v>0</v>
@@ -2842,14 +2689,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="9">
         <f t="shared" ref="J8:J34" si="0">F8-H8</f>
         <v>0</v>
@@ -2857,14 +2704,14 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2872,14 +2719,14 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2887,14 +2734,14 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2902,14 +2749,14 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="31"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2917,14 +2764,14 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2932,14 +2779,14 @@
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2947,14 +2794,14 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2962,14 +2809,14 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2977,14 +2824,14 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2992,14 +2839,14 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3007,14 +2854,14 @@
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="31"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3022,14 +2869,14 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3037,14 +2884,14 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3052,14 +2899,14 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3067,14 +2914,14 @@
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3082,14 +2929,14 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3097,14 +2944,14 @@
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3112,14 +2959,14 @@
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3127,14 +2974,14 @@
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3142,14 +2989,14 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3157,14 +3004,14 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3172,14 +3019,14 @@
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="31"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3187,14 +3034,14 @@
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="31"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3202,14 +3049,14 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="31"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3217,14 +3064,14 @@
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3232,14 +3079,14 @@
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="31"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3247,6 +3094,105 @@
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:G34"/>
@@ -3271,109 +3217,9 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="88" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3400,115 +3246,115 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="32" t="s">
+      <c r="C6" s="15"/>
+      <c r="D6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="32" t="s">
+      <c r="E6" s="25"/>
+      <c r="F6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="33"/>
-      <c r="H6" s="32" t="s">
+      <c r="G6" s="25"/>
+      <c r="H6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="33"/>
+      <c r="I6" s="25"/>
       <c r="J6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="30"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="30"/>
-      <c r="I7" s="31"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="17"/>
       <c r="J7" s="9">
         <f>F7-H7</f>
         <v>0</v>
@@ -3516,14 +3362,14 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="31"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="17"/>
       <c r="J8" s="9">
         <f t="shared" ref="J8:J34" si="0">F8-H8</f>
         <v>0</v>
@@ -3531,14 +3377,14 @@
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="30"/>
-      <c r="I9" s="31"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="17"/>
       <c r="J9" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3546,14 +3392,14 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
       <c r="J10" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3561,14 +3407,14 @@
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="30"/>
-      <c r="I11" s="31"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17"/>
       <c r="J11" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3576,14 +3422,14 @@
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="30"/>
-      <c r="I12" s="31"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17"/>
       <c r="J12" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3591,14 +3437,14 @@
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="30"/>
-      <c r="I13" s="31"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17"/>
       <c r="J13" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3606,14 +3452,14 @@
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="30"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="31"/>
-      <c r="H14" s="30"/>
-      <c r="I14" s="31"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17"/>
       <c r="J14" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3621,14 +3467,14 @@
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="31"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="17"/>
       <c r="J15" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3636,14 +3482,14 @@
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="31"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="17"/>
       <c r="J16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3651,14 +3497,14 @@
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="31"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="17"/>
       <c r="J17" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3666,14 +3512,14 @@
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="31"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="17"/>
       <c r="J18" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3681,14 +3527,14 @@
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="31"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="17"/>
       <c r="J19" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3696,14 +3542,14 @@
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="30"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="30"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="30"/>
-      <c r="I20" s="31"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="17"/>
       <c r="J20" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3711,14 +3557,14 @@
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="31"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="31"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
       <c r="J21" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3726,14 +3572,14 @@
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="31"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="31"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="17"/>
       <c r="J22" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3741,14 +3587,14 @@
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="30"/>
-      <c r="I23" s="31"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3756,14 +3602,14 @@
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="31"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3771,14 +3617,14 @@
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="30"/>
-      <c r="I25" s="31"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3786,14 +3632,14 @@
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="30"/>
-      <c r="E26" s="31"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30"/>
-      <c r="I26" s="31"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3801,14 +3647,14 @@
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="30"/>
-      <c r="I27" s="31"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16"/>
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3816,14 +3662,14 @@
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="30"/>
-      <c r="I28" s="31"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3831,14 +3677,14 @@
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="30"/>
-      <c r="I29" s="31"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3846,14 +3692,14 @@
     </row>
     <row r="30" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="30"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="30"/>
-      <c r="I30" s="31"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3861,14 +3707,14 @@
     </row>
     <row r="31" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="30"/>
-      <c r="I31" s="31"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3876,14 +3722,14 @@
     </row>
     <row r="32" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="31"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3891,14 +3737,14 @@
     </row>
     <row r="33" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="30"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3906,14 +3752,14 @@
     </row>
     <row r="34" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="30"/>
-      <c r="I34" s="31"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3921,6 +3767,105 @@
     </row>
   </sheetData>
   <mergeCells count="123">
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="H12:I12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:G34"/>
@@ -3945,109 +3890,9 @@
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="H12:I12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="87" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4055,7 +3900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
@@ -4074,84 +3919,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="24"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="16"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="18"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27"/>
-      <c r="B3" s="28"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22" t="s">
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="22"/>
+      <c r="J3" s="33"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="34"/>
-      <c r="C6" s="34"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="6" t="s">
         <v>34</v>
       </c>
@@ -4175,11 +4020,11 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="12" t="e">
         <f ca="1">IF(J23=0,"n","s")</f>
         <v>#DIV/0!</v>
@@ -4211,11 +4056,11 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="12" t="e">
         <f t="shared" ref="D8:D19" ca="1" si="0">IF(J24=0,"n","s")</f>
         <v>#DIV/0!</v>
@@ -4247,11 +4092,11 @@
       <c r="L8" s="11"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4283,11 +4128,11 @@
       <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4319,11 +4164,11 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="34"/>
-      <c r="C11" s="34"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4355,11 +4200,11 @@
       <c r="L11" s="11"/>
     </row>
     <row r="12" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="34"/>
-      <c r="C12" s="34"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4391,11 +4236,11 @@
       <c r="L12" s="11"/>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4427,11 +4272,11 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4463,11 +4308,11 @@
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4499,11 +4344,11 @@
       <c r="L15" s="11"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="34" t="s">
+      <c r="A16" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4535,11 +4380,11 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="34" t="s">
+      <c r="A17" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="34"/>
-      <c r="C17" s="34"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4571,11 +4416,11 @@
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4607,11 +4452,11 @@
       <c r="L18" s="11"/>
     </row>
     <row r="19" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+      <c r="A19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="12" t="e">
         <f t="shared" ca="1" si="0"/>
         <v>#DIV/0!</v>
@@ -4643,67 +4488,67 @@
       <c r="L19" s="11"/>
     </row>
     <row r="20" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="29"/>
+      <c r="C20" s="23"/>
       <c r="D20" s="40"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
+      <c r="A21" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="22"/>
+      <c r="J21" s="22"/>
     </row>
     <row r="22" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="32" t="s">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="32" t="s">
+      <c r="E22" s="25"/>
+      <c r="F22" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="33"/>
-      <c r="H22" s="32" t="s">
+      <c r="G22" s="25"/>
+      <c r="H22" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="33"/>
+      <c r="I22" s="25"/>
       <c r="J22" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B23" s="34"/>
-      <c r="C23" s="34"/>
-      <c r="D23" s="30">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="16">
         <f ca="1">Resumo!J7</f>
         <v>0</v>
       </c>
-      <c r="E23" s="31"/>
-      <c r="F23" s="30"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="30">
+      <c r="E23" s="17"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="16">
         <v>8</v>
       </c>
-      <c r="I23" s="31"/>
+      <c r="I23" s="17"/>
       <c r="J23" s="9" t="e">
         <f ca="1">(D23/F23)/H23</f>
         <v>#DIV/0!</v>
@@ -4711,22 +4556,22 @@
       <c r="L23" s="11"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="34" t="s">
+      <c r="A24" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="30">
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="16">
         <f ca="1">Resumo!J8</f>
         <v>0</v>
       </c>
-      <c r="E24" s="31"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="30">
+      <c r="E24" s="17"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="16">
         <v>8</v>
       </c>
-      <c r="I24" s="31"/>
+      <c r="I24" s="17"/>
       <c r="J24" s="9" t="e">
         <f t="shared" ref="J24:J35" ca="1" si="7">(D24/F24)/H24</f>
         <v>#DIV/0!</v>
@@ -4734,22 +4579,22 @@
       <c r="L24" s="11"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
-      <c r="D25" s="30">
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16">
         <f ca="1">Resumo!J9</f>
         <v>0</v>
       </c>
-      <c r="E25" s="31"/>
-      <c r="F25" s="30"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="30">
+      <c r="E25" s="17"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="16">
         <v>8</v>
       </c>
-      <c r="I25" s="31"/>
+      <c r="I25" s="17"/>
       <c r="J25" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4757,22 +4602,22 @@
       <c r="L25" s="11"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="34" t="s">
+      <c r="A26" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="30">
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="16">
         <f ca="1">Resumo!J10</f>
         <v>0</v>
       </c>
-      <c r="E26" s="31"/>
-      <c r="F26" s="30"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="30">
+      <c r="E26" s="17"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="16">
         <v>8</v>
       </c>
-      <c r="I26" s="31"/>
+      <c r="I26" s="17"/>
       <c r="J26" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4780,22 +4625,22 @@
       <c r="L26" s="11"/>
     </row>
     <row r="27" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="A27" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="30">
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="16">
         <f ca="1">Resumo!J11</f>
         <v>0</v>
       </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="30"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="30">
+      <c r="E27" s="17"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="16">
         <v>8</v>
       </c>
-      <c r="I27" s="31"/>
+      <c r="I27" s="17"/>
       <c r="J27" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4803,22 +4648,22 @@
       <c r="L27" s="11"/>
     </row>
     <row r="28" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="30">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="16">
         <f ca="1">Resumo!J12</f>
         <v>0</v>
       </c>
-      <c r="E28" s="31"/>
-      <c r="F28" s="30"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="30">
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="16">
         <v>8</v>
       </c>
-      <c r="I28" s="31"/>
+      <c r="I28" s="17"/>
       <c r="J28" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4826,22 +4671,22 @@
       <c r="L28" s="11"/>
     </row>
     <row r="29" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="30">
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="16">
         <f ca="1">Resumo!J13</f>
         <v>0</v>
       </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="30"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="30">
+      <c r="E29" s="17"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="16">
         <v>8</v>
       </c>
-      <c r="I29" s="31"/>
+      <c r="I29" s="17"/>
       <c r="J29" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4849,22 +4694,22 @@
       <c r="L29" s="11"/>
     </row>
     <row r="30" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="34" t="s">
+      <c r="A30" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="30">
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="16">
         <f ca="1">Resumo!J14</f>
         <v>0</v>
       </c>
-      <c r="E30" s="31"/>
-      <c r="F30" s="30"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="30">
+      <c r="E30" s="17"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="16">
         <v>8</v>
       </c>
-      <c r="I30" s="31"/>
+      <c r="I30" s="17"/>
       <c r="J30" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4872,22 +4717,22 @@
       <c r="L30" s="11"/>
     </row>
     <row r="31" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="34" t="s">
+      <c r="A31" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="30">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16">
         <f ca="1">Resumo!J15</f>
         <v>0</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="30">
+      <c r="E31" s="17"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="16">
         <v>8</v>
       </c>
-      <c r="I31" s="31"/>
+      <c r="I31" s="17"/>
       <c r="J31" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4895,22 +4740,22 @@
       <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34" t="s">
+      <c r="A32" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="30">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="16">
         <f ca="1">Resumo!J16</f>
         <v>0</v>
       </c>
-      <c r="E32" s="31"/>
-      <c r="F32" s="30"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="30">
+      <c r="E32" s="17"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="16">
         <v>8</v>
       </c>
-      <c r="I32" s="31"/>
+      <c r="I32" s="17"/>
       <c r="J32" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4918,22 +4763,22 @@
       <c r="L32" s="11"/>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="30">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="16">
         <f ca="1">Resumo!J17</f>
         <v>0</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="30"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="30">
+      <c r="E33" s="17"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="16">
         <v>8</v>
       </c>
-      <c r="I33" s="31"/>
+      <c r="I33" s="17"/>
       <c r="J33" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4941,22 +4786,22 @@
       <c r="L33" s="11"/>
     </row>
     <row r="34" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="34" t="s">
+      <c r="A34" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="30">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="16">
         <f ca="1">Resumo!J18</f>
         <v>0</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="30"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="30">
+      <c r="E34" s="17"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="16">
         <v>8</v>
       </c>
-      <c r="I34" s="31"/>
+      <c r="I34" s="17"/>
       <c r="J34" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4964,22 +4809,22 @@
       <c r="L34" s="11"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="34" t="s">
+      <c r="A35" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="30">
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="16">
         <f ca="1">Resumo!J19</f>
         <v>0</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="30">
+      <c r="E35" s="17"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="16">
         <v>8</v>
       </c>
-      <c r="I35" s="31"/>
+      <c r="I35" s="17"/>
       <c r="J35" s="9" t="e">
         <f t="shared" ca="1" si="7"/>
         <v>#DIV/0!</v>
@@ -4988,6 +4833,74 @@
     </row>
   </sheetData>
   <mergeCells count="80">
+    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A1:B3"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H32:I32"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="F35:G35"/>
@@ -5000,74 +4913,6 @@
     <mergeCell ref="D34:E34"/>
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="H34:I34"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="A21:J21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A5:J5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A1:B3"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="C4:I4"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:J19 D23:J35">
     <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
@@ -5084,6 +4929,5 @@
   </conditionalFormatting>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125978" footer="0.31496062992125978"/>
   <pageSetup paperSize="9" scale="86" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>